<commit_message>
export version 1.3 for windows 4.3.1
</commit_message>
<xml_diff>
--- a/assets/files/ware-list.xlsx
+++ b/assets/files/ware-list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MLG GRAND\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DDD7A9B4-F44F-4772-A06F-684231EAC87F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60D3ABF6-2BB8-4E64-8BBC-16CBC00787C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8160" yWindow="94" windowWidth="24686" windowHeight="13595" xr2:uid="{E9798EFD-8989-453B-B0BB-A864599C601D}"/>
+    <workbookView xWindow="2983" yWindow="874" windowWidth="15291" windowHeight="17640" xr2:uid="{E9798EFD-8989-453B-B0BB-A864599C601D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>#</t>
   </si>
@@ -57,6 +57,12 @@
   </si>
   <si>
     <t>توضیحات</t>
+  </si>
+  <si>
+    <t>شناسه</t>
+  </si>
+  <si>
+    <t>گروه</t>
   </si>
 </sst>
 </file>
@@ -92,8 +98,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -408,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69964EF4-B017-4940-8781-2DAF6844D92A}">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A10"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -419,14 +427,14 @@
     <col min="1" max="1" width="5.07421875" customWidth="1"/>
     <col min="2" max="2" width="16.84375" customWidth="1"/>
     <col min="3" max="3" width="10.3828125" customWidth="1"/>
-    <col min="4" max="4" width="7.69140625" customWidth="1"/>
+    <col min="4" max="4" width="7.69140625" style="1" customWidth="1"/>
     <col min="5" max="5" width="8.53515625" customWidth="1"/>
-    <col min="6" max="6" width="10.3046875" customWidth="1"/>
-    <col min="7" max="7" width="11.3828125" customWidth="1"/>
-    <col min="8" max="8" width="23.84375" customWidth="1"/>
+    <col min="6" max="6" width="10.3046875" style="2" customWidth="1"/>
+    <col min="7" max="8" width="11.3828125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="23.84375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -449,10 +457,17 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" t="s">
         <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
export version 4.4.1 for bazaar new sale field added
</commit_message>
<xml_diff>
--- a/assets/files/ware-list.xlsx
+++ b/assets/files/ware-list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MLG GRAND\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60D3ABF6-2BB8-4E64-8BBC-16CBC00787C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74BD6819-A20E-4BB9-A564-4CB659263E66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2983" yWindow="874" windowWidth="15291" windowHeight="17640" xr2:uid="{E9798EFD-8989-453B-B0BB-A864599C601D}"/>
+    <workbookView xWindow="8229" yWindow="0" windowWidth="24685" windowHeight="13594" xr2:uid="{E9798EFD-8989-453B-B0BB-A864599C601D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>#</t>
   </si>
@@ -63,16 +63,28 @@
   </si>
   <si>
     <t>گروه</t>
+  </si>
+  <si>
+    <t>فروش 2</t>
+  </si>
+  <si>
+    <t>فروش 3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -416,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69964EF4-B017-4940-8781-2DAF6844D92A}">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -431,10 +443,10 @@
     <col min="5" max="5" width="8.53515625" customWidth="1"/>
     <col min="6" max="6" width="10.3046875" style="2" customWidth="1"/>
     <col min="7" max="8" width="11.3828125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="23.84375" customWidth="1"/>
+    <col min="9" max="9" width="11.15234375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -456,17 +468,24 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>
 </worksheet>

</xml_diff>